<commit_message>
2.1.2 Finish reading The Course for 12 and 2/5 section, paid more attention to the static/dynamic board texture and bet turns more
</commit_message>
<xml_diff>
--- a/DesciplinePokerAtheletes.xlsx
+++ b/DesciplinePokerAtheletes.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="13">
   <si>
     <t>Date</t>
   </si>
@@ -47,6 +47,9 @@
   </si>
   <si>
     <t>Sat</t>
+  </si>
+  <si>
+    <t>Mon</t>
   </si>
 </sst>
 </file>
@@ -234,7 +237,7 @@
         <v>0.0</v>
       </c>
       <c r="H3" s="1">
-        <v>362.0</v>
+        <v>363.0</v>
       </c>
     </row>
     <row r="4">
@@ -286,7 +289,7 @@
         <v>0.0</v>
       </c>
       <c r="H5" s="1">
-        <v>415.0</v>
+        <v>416.0</v>
       </c>
     </row>
     <row r="6">
@@ -338,7 +341,7 @@
         <v>500.0</v>
       </c>
       <c r="H7" s="1">
-        <v>629.0</v>
+        <v>630.0</v>
       </c>
     </row>
     <row r="8">
@@ -389,8 +392,8 @@
       <c r="G9" s="1">
         <v>0.0</v>
       </c>
-      <c r="H9" s="9">
-        <v>346.0</v>
+      <c r="H9" s="6">
+        <v>347.0</v>
       </c>
     </row>
     <row r="10">
@@ -441,8 +444,8 @@
       <c r="G11" s="1">
         <v>0.0</v>
       </c>
-      <c r="H11" s="9">
-        <v>749.0</v>
+      <c r="H11" s="6">
+        <v>750.0</v>
       </c>
     </row>
     <row r="12">
@@ -493,8 +496,8 @@
       <c r="G13" s="1">
         <v>0.0</v>
       </c>
-      <c r="H13" s="9">
-        <v>439.0</v>
+      <c r="H13" s="6">
+        <v>440.0</v>
       </c>
       <c r="I13" s="1"/>
       <c r="J13" s="11"/>
@@ -548,7 +551,85 @@
         <v>0.0</v>
       </c>
       <c r="H15" s="1">
-        <v>604.0</v>
+        <v>605.0</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="12">
+        <v>43433.0</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C16" s="1">
+        <v>2.0</v>
+      </c>
+      <c r="D16" s="13">
+        <v>43433.86388888889</v>
+      </c>
+      <c r="E16" s="13">
+        <v>43434.120833333334</v>
+      </c>
+      <c r="F16" s="1">
+        <v>500.0</v>
+      </c>
+      <c r="G16" s="1">
+        <v>0.0</v>
+      </c>
+      <c r="H16" s="1">
+        <v>693.0</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="12">
+        <v>43434.0</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C17" s="1">
+        <v>3.0</v>
+      </c>
+      <c r="D17" s="13">
+        <v>43434.99930555555</v>
+      </c>
+      <c r="E17" s="13">
+        <v>43435.15625</v>
+      </c>
+      <c r="F17" s="1">
+        <v>300.0</v>
+      </c>
+      <c r="G17" s="1">
+        <v>0.0</v>
+      </c>
+      <c r="H17" s="1">
+        <v>724.0</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="12">
+        <v>43436.0</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C18" s="1">
+        <v>2.0</v>
+      </c>
+      <c r="D18" s="13">
+        <v>43437.59375</v>
+      </c>
+      <c r="E18" s="13">
+        <v>43437.80902777778</v>
+      </c>
+      <c r="F18" s="1">
+        <v>300.0</v>
+      </c>
+      <c r="G18" s="1">
+        <v>0.0</v>
+      </c>
+      <c r="H18" s="1">
+        <v>851.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Data set updated at Jan 3rd
</commit_message>
<xml_diff>
--- a/DesciplinePokerAtheletes.xlsx
+++ b/DesciplinePokerAtheletes.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="14">
   <si>
     <t>Date</t>
   </si>
@@ -863,6 +863,35 @@
         <v>1316.0</v>
       </c>
     </row>
+    <row r="25">
+      <c r="A25" s="12">
+        <v>43468.0</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C25" s="1">
+        <v>2.4</v>
+      </c>
+      <c r="D25" s="1">
+        <v>2.0</v>
+      </c>
+      <c r="E25" s="13">
+        <v>43103.94305555556</v>
+      </c>
+      <c r="F25" s="13">
+        <v>43104.26944444444</v>
+      </c>
+      <c r="G25" s="1">
+        <v>1200.0</v>
+      </c>
+      <c r="H25" s="1">
+        <v>0.0</v>
+      </c>
+      <c r="I25" s="1">
+        <v>1400.0</v>
+      </c>
+    </row>
   </sheetData>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Updated by May 1st 2019
</commit_message>
<xml_diff>
--- a/DesciplinePokerAtheletes.xlsx
+++ b/DesciplinePokerAtheletes.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="15">
   <si>
     <t>Date</t>
   </si>
@@ -62,10 +62,11 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <numFmts count="3">
+  <numFmts count="4">
     <numFmt numFmtId="164" formatCode="mmm d"/>
     <numFmt numFmtId="165" formatCode="m/d/yy h:mm"/>
     <numFmt numFmtId="166" formatCode="mmmd"/>
+    <numFmt numFmtId="167" formatCode="mmmm d"/>
   </numFmts>
   <fonts count="4">
     <font>
@@ -102,7 +103,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -143,6 +144,9 @@
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="165" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="167" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
@@ -1156,6 +1160,93 @@
         <v>2820.0</v>
       </c>
     </row>
+    <row r="35">
+      <c r="A35" s="12">
+        <v>43552.0</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C35" s="1">
+        <v>2.8</v>
+      </c>
+      <c r="D35" s="1">
+        <v>3.0</v>
+      </c>
+      <c r="E35" s="13">
+        <v>43552.65277777778</v>
+      </c>
+      <c r="F35" s="13">
+        <v>43553.125</v>
+      </c>
+      <c r="G35" s="1">
+        <v>1000.0</v>
+      </c>
+      <c r="H35" s="1">
+        <v>0.0</v>
+      </c>
+      <c r="I35" s="1">
+        <v>342.0</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="12">
+        <v>43581.0</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C36" s="1">
+        <v>3.0</v>
+      </c>
+      <c r="D36" s="1">
+        <v>3.0</v>
+      </c>
+      <c r="E36" s="13">
+        <v>43581.75</v>
+      </c>
+      <c r="F36" s="13">
+        <v>43582.28472222222</v>
+      </c>
+      <c r="G36" s="1">
+        <v>520.0</v>
+      </c>
+      <c r="H36" s="1">
+        <v>0.0</v>
+      </c>
+      <c r="I36" s="1">
+        <v>274.0</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="14">
+        <v>43586.0</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C37" s="1">
+        <v>2.0</v>
+      </c>
+      <c r="D37" s="1">
+        <v>2.0</v>
+      </c>
+      <c r="E37" s="13">
+        <v>43586.575</v>
+      </c>
+      <c r="F37" s="13">
+        <v>43586.947916666664</v>
+      </c>
+      <c r="G37" s="1">
+        <v>260.0</v>
+      </c>
+      <c r="H37" s="1">
+        <v>0.0</v>
+      </c>
+      <c r="I37" s="1">
+        <v>1233.0</v>
+      </c>
+    </row>
   </sheetData>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Updated Early Jan 2020
</commit_message>
<xml_diff>
--- a/DesciplinePokerAtheletes.xlsx
+++ b/DesciplinePokerAtheletes.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="17">
   <si>
     <t>Date</t>
   </si>
@@ -60,16 +60,20 @@
   <si>
     <t>Feb</t>
   </si>
+  <si>
+    <t>Sun</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <numFmts count="4">
+  <numFmts count="5">
     <numFmt numFmtId="164" formatCode="mmm d"/>
     <numFmt numFmtId="165" formatCode="m/d/yy h:mm"/>
     <numFmt numFmtId="166" formatCode="mmmd"/>
     <numFmt numFmtId="167" formatCode="mmmm d"/>
+    <numFmt numFmtId="168" formatCode="mm/dd/yy h:mm"/>
   </numFmts>
   <fonts count="4">
     <font>
@@ -106,7 +110,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="17">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -152,6 +156,12 @@
     <xf borderId="0" fillId="0" fontId="1" numFmtId="167" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="168" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="3" numFmtId="165" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
@@ -1945,6 +1955,344 @@
         <v>768.0</v>
       </c>
     </row>
+    <row r="63">
+      <c r="A63" s="12">
+        <v>43710.0</v>
+      </c>
+      <c r="B63" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C63" s="1">
+        <v>2.6</v>
+      </c>
+      <c r="E63" s="13">
+        <v>43710.384722222225</v>
+      </c>
+      <c r="F63" s="13">
+        <v>43710.62013888889</v>
+      </c>
+      <c r="G63" s="1">
+        <v>1280.0</v>
+      </c>
+      <c r="H63" s="1">
+        <v>0.0</v>
+      </c>
+      <c r="I63" s="1">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" s="12">
+        <v>44085.0</v>
+      </c>
+      <c r="B64" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C64" s="1">
+        <v>3.0</v>
+      </c>
+      <c r="E64" s="13">
+        <v>43720.08611111111</v>
+      </c>
+      <c r="F64" s="13">
+        <v>43720.291666666664</v>
+      </c>
+      <c r="G64" s="1">
+        <v>500.0</v>
+      </c>
+      <c r="H64" s="1">
+        <v>0.0</v>
+      </c>
+      <c r="I64" s="1">
+        <v>366.0</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" s="12">
+        <v>44087.0</v>
+      </c>
+      <c r="B65" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C65" s="1">
+        <v>3.0</v>
+      </c>
+      <c r="E65" s="13">
+        <v>43721.70763888889</v>
+      </c>
+      <c r="F65" s="13">
+        <v>43721.938888888886</v>
+      </c>
+      <c r="G65" s="1">
+        <v>300.0</v>
+      </c>
+      <c r="H65" s="1">
+        <v>0.0</v>
+      </c>
+      <c r="I65" s="1">
+        <v>894.0</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" s="12">
+        <v>44094.0</v>
+      </c>
+      <c r="B66" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C66" s="1">
+        <v>3.0</v>
+      </c>
+      <c r="E66" s="13">
+        <v>43728.92013888889</v>
+      </c>
+      <c r="F66" s="13">
+        <v>43729.083333333336</v>
+      </c>
+      <c r="G66" s="1">
+        <v>200.0</v>
+      </c>
+      <c r="H66" s="1">
+        <v>0.0</v>
+      </c>
+      <c r="I66" s="1">
+        <v>509.0</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" s="12">
+        <v>44113.0</v>
+      </c>
+      <c r="B67" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C67" s="1">
+        <v>3.0</v>
+      </c>
+      <c r="E67" s="15">
+        <v>43747.48819444444</v>
+      </c>
+      <c r="F67" s="15">
+        <v>43747.666666666664</v>
+      </c>
+      <c r="G67" s="1">
+        <v>360.0</v>
+      </c>
+      <c r="H67" s="1">
+        <v>0.0</v>
+      </c>
+      <c r="I67" s="1">
+        <v>800.0</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" s="12">
+        <v>44136.0</v>
+      </c>
+      <c r="B68" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C68" s="1">
+        <v>3.0</v>
+      </c>
+      <c r="E68" s="15">
+        <v>43771.01111111111</v>
+      </c>
+      <c r="F68" s="15">
+        <v>43771.114583333336</v>
+      </c>
+      <c r="G68" s="1">
+        <v>600.0</v>
+      </c>
+      <c r="H68" s="1">
+        <v>0.0</v>
+      </c>
+      <c r="I68" s="1">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" s="12">
+        <v>44143.0</v>
+      </c>
+      <c r="B69" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C69" s="1">
+        <v>3.0</v>
+      </c>
+      <c r="E69" s="16">
+        <v>43777.694444444445</v>
+      </c>
+      <c r="F69" s="13">
+        <v>43778.125</v>
+      </c>
+      <c r="G69" s="1">
+        <v>300.0</v>
+      </c>
+      <c r="H69" s="1">
+        <v>0.0</v>
+      </c>
+      <c r="I69" s="1">
+        <v>699.0</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" s="12">
+        <v>44153.0</v>
+      </c>
+      <c r="B70" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C70" s="1">
+        <v>3.0</v>
+      </c>
+      <c r="E70" s="13">
+        <v>43788.03472222222</v>
+      </c>
+      <c r="F70" s="13">
+        <v>43788.20625</v>
+      </c>
+      <c r="G70" s="1">
+        <v>350.0</v>
+      </c>
+      <c r="H70" s="1">
+        <v>0.0</v>
+      </c>
+      <c r="I70" s="1">
+        <v>1231.0</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" s="12">
+        <v>44157.0</v>
+      </c>
+      <c r="B71" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C71" s="1">
+        <v>2.0</v>
+      </c>
+      <c r="E71" s="13">
+        <v>43791.71875</v>
+      </c>
+      <c r="F71" s="13">
+        <v>43791.944444444445</v>
+      </c>
+      <c r="G71" s="1">
+        <v>960.0</v>
+      </c>
+      <c r="H71" s="1">
+        <v>0.0</v>
+      </c>
+      <c r="I71" s="1">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" s="12">
+        <v>44160.0</v>
+      </c>
+      <c r="B72" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C72" s="1">
+        <v>2.0</v>
+      </c>
+      <c r="E72" s="13">
+        <v>43794.913194444445</v>
+      </c>
+      <c r="F72" s="13">
+        <v>43795.02291666667</v>
+      </c>
+      <c r="G72" s="1">
+        <v>500.0</v>
+      </c>
+      <c r="H72" s="1">
+        <v>0.0</v>
+      </c>
+      <c r="I72" s="1">
+        <v>908.0</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" s="12">
+        <v>44164.0</v>
+      </c>
+      <c r="B73" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C73" s="1">
+        <v>3.0</v>
+      </c>
+      <c r="E73" s="13">
+        <v>43799.01111111111</v>
+      </c>
+      <c r="F73" s="13">
+        <v>43799.25347222222</v>
+      </c>
+      <c r="G73" s="1">
+        <v>700.0</v>
+      </c>
+      <c r="H73" s="1">
+        <v>0.0</v>
+      </c>
+      <c r="I73" s="1">
+        <v>784.0</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" s="12">
+        <v>44173.0</v>
+      </c>
+      <c r="B74" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C74" s="1">
+        <v>3.0</v>
+      </c>
+      <c r="E74" s="15">
+        <v>43807.961805555555</v>
+      </c>
+      <c r="F74" s="15">
+        <v>43808.15277777778</v>
+      </c>
+      <c r="G74" s="1">
+        <v>600.0</v>
+      </c>
+      <c r="H74" s="1">
+        <v>0.0</v>
+      </c>
+      <c r="I74" s="1">
+        <v>382.0</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" s="12">
+        <v>43834.0</v>
+      </c>
+      <c r="B75" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C75" s="1">
+        <v>3.0</v>
+      </c>
+      <c r="E75" s="15">
+        <v>43835.118055555555</v>
+      </c>
+      <c r="F75" s="15">
+        <v>43835.552083333336</v>
+      </c>
+      <c r="G75" s="1">
+        <v>300.0</v>
+      </c>
+      <c r="H75" s="1">
+        <v>0.0</v>
+      </c>
+      <c r="I75" s="1">
+        <v>1263.0</v>
+      </c>
+    </row>
   </sheetData>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Updated by Early Jan
</commit_message>
<xml_diff>
--- a/DesciplinePokerAtheletes.xlsx
+++ b/DesciplinePokerAtheletes.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="16">
   <si>
     <t>Date</t>
   </si>
@@ -59,9 +59,6 @@
   </si>
   <si>
     <t>Feb</t>
-  </si>
-  <si>
-    <t>Sun</t>
   </si>
 </sst>
 </file>
@@ -1960,7 +1957,7 @@
         <v>43710.0</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C63" s="1">
         <v>2.6</v>

</xml_diff>